<commit_message>
Excel for Manual Testing Classwork
</commit_message>
<xml_diff>
--- a/Manual Software Testing.xlsx
+++ b/Manual Software Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Arnab Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0D23D6-0840-4B4F-BCE5-7F9A079F4CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453C536C-2971-4510-87FB-8A68043A8FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6F988C16-CC91-4359-BFDC-ED1BB7A0CE5A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Project Name:</t>
   </si>
@@ -158,9 +158,6 @@
     <t>TC_ERP_Login_002</t>
   </si>
   <si>
-    <t>Rnter valid user name and one invalid password</t>
-  </si>
-  <si>
     <t>1. Enter valid username
 2. Enter invalid password
 3. Click on the Login Button</t>
@@ -180,6 +177,39 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_003</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_004</t>
+  </si>
+  <si>
+    <t>Enter valid user name and one invalid password</t>
+  </si>
+  <si>
+    <t>Enter invalid user name and one valid password</t>
+  </si>
+  <si>
+    <t>Enter invalid user name and one invalid password</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter invalid password
+3. Click on the Login Button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter valid password
+3. Click on the Login Button</t>
+  </si>
+  <si>
+    <t>Username: xxxx@erp.com
+Password: P@asw0rd</t>
+  </si>
+  <si>
+    <t>Username: xxxx@erp.com
+Password: xxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -234,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -347,11 +377,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -384,11 +510,357 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mmm/yyyy\ \(ddd\)"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -399,6 +871,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F83C955-4F71-4A02-8F82-AED0B3268E6C}" name="Table1" displayName="Table1" ref="A9:N13" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{6F1C4EF0-64E9-466D-A03E-0C79E40A1879}" name="Test Scenario ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{BCBD0EEF-6F26-49B4-9E38-49B0AFF67D40}" name="Test Scenario Description" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{5C33D355-02F7-4F10-A7A7-1181AC5BEADD}" name="Test Case_x000a_ID" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{813992A4-FAD5-400D-AD27-5CE7B71913F7}" name="Test Case_x000a_Description" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{C92E5DAC-5199-4A34-8B15-054A360A219C}" name="Test Steps" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{D8D71509-02F3-4236-BA70-2D4BB170DB71}" name="Pre-Conditions" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{B0025A32-155F-4AAE-9664-B684C9035542}" name="Test Data" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{C6859671-5F2C-4060-B8F0-EA52556A65A3}" name="Post-Conditions" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{93BB7EDC-7CD7-4068-AF72-196AA6755514}" name="Expected Result" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{87396A2B-4557-4DDC-BE07-8D787C2A0CD2}" name="Actual Result" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{410EFB28-2AD3-49FC-B3CB-F3E7C4E7F3A3}" name="Status" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{D022FC1E-3D2F-4547-A9B2-83FC3A2598E2}" name="Executed By" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{8654FE21-BAD9-4E67-BBCB-F043B10208AE}" name="Excution Date" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{0181C038-4BE0-4DB2-B352-8B33A4D1174B}" name="Comments_x000a_(If Any)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -720,21 +1214,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A846D1A5-0BBE-4E86-9CD8-4A8F1165B7D0}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="6" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
     <col min="9" max="9" width="17.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -788,51 +1284,51 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="9" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="N9" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -871,12 +1367,12 @@
       <c r="M10" s="15">
         <v>45113</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="N10" s="19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="9" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -886,73 +1382,134 @@
         <v>37</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>34</v>
       </c>
       <c r="M11" s="15">
-        <v>45114</v>
-      </c>
-      <c r="N11" s="11" t="s">
+        <v>45117</v>
+      </c>
+      <c r="N11" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
+    <row r="12" spans="1:14" s="8" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="15">
+        <v>45120</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
+    <row r="13" spans="1:14" s="8" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="27">
+        <v>45120</v>
+      </c>
+      <c r="N13" s="28" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>